<commit_message>
create conversion2_aa3 (update of conversion_aa3) create calc_newlm in calb_aa3 (function for recalculating linear regression)
</commit_message>
<xml_diff>
--- a/Data/raw/181009A.xlsx
+++ b/Data/raw/181009A.xlsx
@@ -14,6 +14,8 @@
   <definedNames>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Area" vbProcedure="false">data!$A$1:$F$50</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Area" vbProcedure="false">data!$A$1:$F$50</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Area_0" vbProcedure="false">data!$A$1:$F$50</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Area_0_0" vbProcedure="false">data!$A$1:$F$50</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">data!$C$1:$C$1</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
@@ -166,8 +168,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -212,21 +218,21 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="10.7323943661972"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.67136150234742"/>
   </cols>
   <sheetData>
     <row r="4" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+      <c r="A7" s="1" t="s">
         <v>2</v>
       </c>
     </row>
@@ -249,139 +255,139 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D14" activeCellId="0" sqref="D14"/>
+      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.1408450704225"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.9859154929577"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="23.0892018779343"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.1032863849765"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="9.53990610328638"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="23.5258215962441"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="10.7323943661972"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="21.8967136150235"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="14.5258215962441"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="23.9577464788732"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="18.7558685446009"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="9.97183098591549"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="24.5023474178404"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.67136150234742"/>
   </cols>
   <sheetData>
-    <row r="1" s="2" customFormat="true" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
+    <row r="1" s="3" customFormat="true" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="3" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="0" t="s">
+      <c r="A2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="1" t="n">
-        <v>43382.5944444444</v>
-      </c>
-      <c r="D2" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" s="4" t="s">
+      <c r="C2" s="2" t="n">
+        <v>43382.5944444444</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="5" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="0" t="s">
+      <c r="A3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="1" t="n">
-        <v>43301.4013888889</v>
-      </c>
-      <c r="D3" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="4" t="s">
+      <c r="C3" s="2" t="n">
+        <v>43382.5944444444</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="5" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="0" t="s">
+      <c r="A4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="1" t="n">
-        <v>43301.4013888889</v>
-      </c>
-      <c r="D4" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4" s="4" t="s">
+      <c r="C4" s="2" t="n">
+        <v>43382.5944444444</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="5" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="0" t="s">
+      <c r="A5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="1" t="n">
-        <v>43301.4013888889</v>
-      </c>
-      <c r="D5" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="E5" s="4" t="s">
+      <c r="C5" s="2" t="n">
+        <v>43382.5944444444</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="5" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="0" t="s">
+      <c r="A6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="1" t="n">
-        <v>43301.4013888889</v>
-      </c>
-      <c r="D6" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="E6" s="4" t="s">
+      <c r="C6" s="2" t="n">
+        <v>43382.5944444444</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" s="5" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" s="0" t="s">
+      <c r="A7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="1" t="n">
-        <v>43301.4145833333</v>
-      </c>
-      <c r="D7" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="E7" s="4" t="s">
+      <c r="C7" s="2" t="n">
+        <v>43382.5944444444</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" s="5" t="s">
         <v>18</v>
       </c>
     </row>

</xml_diff>